<commit_message>
removed name pop up at login, and added exception handling for gsuite error, and changed rules
</commit_message>
<xml_diff>
--- a/Project2Final/Rules.xlsx
+++ b/Project2Final/Rules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagib\Documents\Revature\JewlzAndTheBoyz-EmailCategorizationBot-P2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ohhey\Desktop\Revature_Workspace\JewlzAndTheBoyz-EmailCategorizationBot-P2\Project2Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635F6638-D782-4A75-B41A-9E3B9E7A4924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF98B371-EFE6-43AF-8370-DD20DDEAA7F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34890" yWindow="2100" windowWidth="17280" windowHeight="9030" xr2:uid="{F8A05525-B3EB-4424-9D4D-7345C82E46E0}"/>
+    <workbookView xWindow="61965" yWindow="2895" windowWidth="17280" windowHeight="9000" activeTab="1" xr2:uid="{F8A05525-B3EB-4424-9D4D-7345C82E46E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Julie" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>foleyb25@gmail.com</t>
   </si>
@@ -430,16 +430,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C594C03D-EEF8-416F-BD6B-CF19B76CC1D2}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -468,19 +468,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC671B8-FB17-4529-998D-C1A952BEB850}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="12.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.20703125" customWidth="1"/>
+    <col min="4" max="4" width="10.20703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -494,7 +496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -502,7 +504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -510,7 +512,26 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{EE517172-54FF-4ACF-BB0B-135858D2D6F4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -523,13 +544,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -543,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -551,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>9</v>
       </c>

</xml_diff>